<commit_message>
Edit unstable start figure. Edit lake 1000 and 64 sonde data files. Add interpolation of surface sonde data from lake 207 based on NLA profile.
</commit_message>
<xml_diff>
--- a/SuRGE_Sharepoint/data/NAR/CH4_064_Halls_Pond/dataSheets/surgeData064.xlsx
+++ b/SuRGE_Sharepoint/data/NAR/CH4_064_Halls_Pond/dataSheets/surgeData064.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/SuRGE/Shared Documents/data/NAR/CH4_064_Halls_Pond/dataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="627" documentId="8_{6F7B1609-39B3-461F-8F88-BC510D6E631F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{164F9AFF-1ADE-4A40-A046-F04D712B4D86}"/>
+  <xr:revisionPtr revIDLastSave="628" documentId="8_{6F7B1609-39B3-461F-8F88-BC510D6E631F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38C6A6CE-D50E-4907-BC44-8D9D579170FF}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1391,9 +1391,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1431,7 +1431,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1537,7 +1537,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1679,7 +1679,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1690,84 +1690,83 @@
   <dimension ref="A1:BY17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BU6" sqref="BU6"/>
+      <pane xSplit="2" topLeftCell="AJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BA17" sqref="BA17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9.77734375" customWidth="1"/>
-    <col min="19" max="19" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="12.44140625" customWidth="1"/>
-    <col min="26" max="26" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.109375" customWidth="1"/>
-    <col min="29" max="29" width="8.109375" customWidth="1"/>
-    <col min="30" max="30" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.7109375" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="12.42578125" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.140625" customWidth="1"/>
+    <col min="29" max="29" width="8.140625" customWidth="1"/>
+    <col min="30" max="30" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.88671875" customWidth="1"/>
-    <col min="33" max="33" width="6.44140625" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" customWidth="1"/>
+    <col min="33" max="33" width="6.42578125" customWidth="1"/>
     <col min="34" max="34" width="8" customWidth="1"/>
     <col min="35" max="35" width="6" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="18" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13.77734375" customWidth="1"/>
-    <col min="48" max="49" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.7109375" customWidth="1"/>
+    <col min="48" max="49" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="8" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="6.88671875" customWidth="1"/>
-    <col min="54" max="54" width="7.77734375" customWidth="1"/>
-    <col min="55" max="55" width="8.77734375" customWidth="1"/>
-    <col min="56" max="56" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="6.85546875" customWidth="1"/>
+    <col min="54" max="54" width="7.7109375" customWidth="1"/>
+    <col min="55" max="55" width="8.7109375" customWidth="1"/>
+    <col min="56" max="56" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="11" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.77734375" customWidth="1"/>
+    <col min="58" max="58" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.7109375" customWidth="1"/>
     <col min="63" max="63" width="10" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="14" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="14" customWidth="1"/>
-    <col min="70" max="70" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="73" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="74" max="75" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="73" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="75" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -1858,7 +1857,7 @@
       <c r="BX1" s="34"/>
       <c r="BY1" s="34"/>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>6</v>
       </c>
@@ -2091,7 +2090,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>184</v>
       </c>
@@ -2213,7 +2212,7 @@
         <v>0.56944444444444442</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>184</v>
       </c>
@@ -2314,7 +2313,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>184</v>
       </c>
@@ -2416,7 +2415,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>184</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>184</v>
       </c>
@@ -2622,7 +2621,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>184</v>
       </c>
@@ -2723,7 +2722,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>184</v>
       </c>
@@ -2824,7 +2823,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>184</v>
       </c>
@@ -2926,7 +2925,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>184</v>
       </c>
@@ -3027,7 +3026,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>184</v>
       </c>
@@ -3128,7 +3127,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>184</v>
       </c>
@@ -3230,7 +3229,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>184</v>
       </c>
@@ -3331,7 +3330,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>184</v>
       </c>
@@ -3432,7 +3431,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>184</v>
       </c>
@@ -3521,7 +3520,7 @@
         <v>53.6</v>
       </c>
       <c r="BA16">
-        <v>91.6</v>
+        <v>9.16</v>
       </c>
       <c r="BB16">
         <v>1.24</v>
@@ -3533,7 +3532,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>184</v>
       </c>
@@ -3660,15 +3659,15 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="116.77734375" style="26" customWidth="1"/>
-    <col min="3" max="3" width="49.5546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="26"/>
+    <col min="1" max="1" width="17.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="116.7109375" style="26" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>74</v>
       </c>
@@ -3679,7 +3678,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>6</v>
       </c>
@@ -3690,7 +3689,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>7</v>
       </c>
@@ -3701,7 +3700,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>8</v>
       </c>
@@ -3712,7 +3711,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>9</v>
       </c>
@@ -3723,7 +3722,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>10</v>
       </c>
@@ -3734,7 +3733,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>11</v>
       </c>
@@ -3745,7 +3744,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>12</v>
       </c>
@@ -3756,7 +3755,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>13</v>
       </c>
@@ -3767,7 +3766,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>14</v>
       </c>
@@ -3778,7 +3777,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>15</v>
       </c>
@@ -3789,7 +3788,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>16</v>
       </c>
@@ -3800,7 +3799,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>17</v>
       </c>
@@ -3811,7 +3810,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>18</v>
       </c>
@@ -3819,7 +3818,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>19</v>
       </c>
@@ -3830,7 +3829,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>20</v>
       </c>
@@ -3838,7 +3837,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>21</v>
       </c>
@@ -3849,7 +3848,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>22</v>
       </c>
@@ -3857,7 +3856,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>101</v>
       </c>
@@ -3868,7 +3867,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
         <v>104</v>
       </c>
@@ -3876,7 +3875,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>23</v>
       </c>
@@ -3887,7 +3886,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>24</v>
       </c>
@@ -3898,7 +3897,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>25</v>
       </c>
@@ -3909,7 +3908,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>26</v>
       </c>
@@ -3920,7 +3919,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>27</v>
       </c>
@@ -3931,7 +3930,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
         <v>112</v>
       </c>
@@ -3942,7 +3941,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
         <v>113</v>
       </c>
@@ -3950,7 +3949,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>28</v>
       </c>
@@ -3961,7 +3960,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>29</v>
       </c>
@@ -3972,7 +3971,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>30</v>
       </c>
@@ -3983,7 +3982,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>31</v>
       </c>
@@ -3994,7 +3993,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
         <v>32</v>
       </c>
@@ -4005,7 +4004,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
         <v>33</v>
       </c>
@@ -4016,7 +4015,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>34</v>
       </c>
@@ -4027,7 +4026,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
         <v>35</v>
       </c>
@@ -4038,7 +4037,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
         <v>36</v>
       </c>
@@ -4046,7 +4045,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
         <v>37</v>
       </c>
@@ -4054,7 +4053,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
         <v>38</v>
       </c>
@@ -4062,7 +4061,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
         <v>39</v>
       </c>
@@ -4070,7 +4069,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
         <v>40</v>
       </c>
@@ -4078,7 +4077,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
         <v>41</v>
       </c>
@@ -4086,7 +4085,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
         <v>42</v>
       </c>
@@ -4094,7 +4093,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
         <v>43</v>
       </c>
@@ -4102,7 +4101,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
         <v>44</v>
       </c>
@@ -4110,7 +4109,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
         <v>45</v>
       </c>
@@ -4118,7 +4117,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="26" t="s">
         <v>46</v>
       </c>
@@ -4126,7 +4125,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="26" t="s">
         <v>47</v>
       </c>
@@ -4134,7 +4133,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="26" t="s">
         <v>48</v>
       </c>
@@ -4145,7 +4144,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
         <v>49</v>
       </c>
@@ -4156,7 +4155,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="26" t="s">
         <v>50</v>
       </c>
@@ -4167,7 +4166,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="26" t="s">
         <v>51</v>
       </c>
@@ -4178,7 +4177,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="26" t="s">
         <v>52</v>
       </c>
@@ -4189,7 +4188,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
         <v>53</v>
       </c>
@@ -4200,7 +4199,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
         <v>54</v>
       </c>
@@ -4211,7 +4210,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>55</v>
       </c>
@@ -4219,7 +4218,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
         <v>56</v>
       </c>
@@ -4227,7 +4226,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
         <v>57</v>
       </c>
@@ -4235,7 +4234,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="26" t="s">
         <v>58</v>
       </c>
@@ -4243,7 +4242,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="26" t="s">
         <v>59</v>
       </c>
@@ -4251,7 +4250,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="26" t="s">
         <v>60</v>
       </c>
@@ -4259,7 +4258,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="26" t="s">
         <v>61</v>
       </c>
@@ -4267,7 +4266,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="26" t="s">
         <v>62</v>
       </c>
@@ -4275,7 +4274,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="26" t="s">
         <v>63</v>
       </c>
@@ -4283,7 +4282,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="26" t="s">
         <v>64</v>
       </c>
@@ -4291,7 +4290,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="26" t="s">
         <v>65</v>
       </c>
@@ -4299,7 +4298,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="26" t="s">
         <v>66</v>
       </c>
@@ -4307,7 +4306,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="26" t="s">
         <v>67</v>
       </c>
@@ -4318,7 +4317,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="26" t="s">
         <v>68</v>
       </c>
@@ -4329,7 +4328,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="26" t="s">
         <v>69</v>
       </c>
@@ -4340,7 +4339,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="26" t="s">
         <v>70</v>
       </c>
@@ -4351,7 +4350,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="26" t="s">
         <v>71</v>
       </c>
@@ -4362,7 +4361,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="26" t="s">
         <v>72</v>
       </c>
@@ -4373,7 +4372,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="26" t="s">
         <v>73</v>
       </c>
@@ -4397,17 +4396,17 @@
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="24"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="24"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>5</v>
       </c>
@@ -4423,7 +4422,7 @@
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4457,7 +4456,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>179</v>
       </c>
@@ -4486,7 +4485,7 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>179</v>
       </c>
@@ -4515,7 +4514,7 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>179</v>
       </c>
@@ -4544,7 +4543,7 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>179</v>
       </c>
@@ -4573,7 +4572,7 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>179</v>
       </c>
@@ -4602,7 +4601,7 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>179</v>
       </c>
@@ -4648,14 +4647,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.5546875" customWidth="1"/>
-    <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.5703125" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -4666,7 +4665,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4677,7 +4676,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -4688,7 +4687,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>154</v>
       </c>
@@ -4699,7 +4698,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>155</v>
       </c>
@@ -4710,7 +4709,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>156</v>
       </c>
@@ -4721,7 +4720,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>157</v>
       </c>
@@ -4729,7 +4728,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>158</v>
       </c>
@@ -4740,7 +4739,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>159</v>
       </c>
@@ -4751,7 +4750,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>160</v>
       </c>
@@ -4762,7 +4761,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>161</v>
       </c>
@@ -4779,59 +4778,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-10-21T13:32:44+00:00</Document_x0020_Creation_x0020_Date>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001AF5FC5DD832BE4DBA6B24560DD3ADC0" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d40b3e6283001fb57e5088f84fb23d5e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="8b03727f-4454-4722-b3e6-018d8dcaf2fd" xmlns:ns6="ed970698-2d60-4bab-a048-d9be527522d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aadbb8160917885bdc8cfb32badaafe9" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001AF5FC5DD832BE4DBA6B24560DD3ADC0" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d0c06073aad642fb447e451b4bd3149">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="8b03727f-4454-4722-b3e6-018d8dcaf2fd" xmlns:ns6="ed970698-2d60-4bab-a048-d9be527522d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f347bf1c409ca453852eb5a13773c360" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint.v3"/>
@@ -4877,6 +4825,8 @@
                 <xsd:element ref="ns6:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns6:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns6:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4932,6 +4882,16 @@
           <xsd:enumeration value="Urdu (Islamic Republic of Pakistan)"/>
           <xsd:enumeration value="Vietnamese (Vietnam)"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="45" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="46" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -5300,15 +5260,83 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2020-10-21T13:32:44+00:00</Document_x0020_Creation_x0020_Date>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F4A5FCF-4499-487A-89B0-E215184C11DF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65B7B9C0-18CC-4B70-B381-384210C0B58A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="8b03727f-4454-4722-b3e6-018d8dcaf2fd"/>
+    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5328,7 +5356,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64AF5971-BB1F-4D87-A3D3-C75CDE44C1C9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F4A5FCF-4499-487A-89B0-E215184C11DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>